<commit_message>
Fixed spacing in scrollingplotwidget.py
</commit_message>
<xml_diff>
--- a/lib/VortexTest.xlsx
+++ b/lib/VortexTest.xlsx
@@ -5,21 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayash\Programming\vortex_parser\lib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yash Jain\Programming\SailProj\vortex_parser\vortex_parser\lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF7E14A-C715-402A-B58A-1AF4D8635C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881B01EA-188E-4DAD-8F8D-9E727F7B5A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21345" windowHeight="15600" tabRatio="522" xr2:uid="{93DD1A3E-79F5-40A0-9DE4-B4C0229D9C52}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="522" xr2:uid="{93DD1A3E-79F5-40A0-9DE4-B4C0229D9C52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="AAA">Sheet1!$AMO$13</definedName>
-    <definedName name="Ash">Sheet1!$AMO$13</definedName>
-    <definedName name="YAS">Sheet1!$AMO$12</definedName>
-    <definedName name="Yash">Sheet1!$AMY$16</definedName>
+    <definedName name="AAA">Sheet1!$AMO$14</definedName>
+    <definedName name="Ash">Sheet1!$AMO$14</definedName>
+    <definedName name="YAS">Sheet1!$AMO$13</definedName>
+    <definedName name="Yash">Sheet1!$AMY$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="64">
   <si>
     <t>Bitmask</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>Map:</t>
+  </si>
+  <si>
+    <t>Maps</t>
   </si>
 </sst>
 </file>
@@ -259,7 +262,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -356,6 +359,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -531,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -609,6 +618,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -936,19 +946,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7758D255-7225-412E-BCCB-5D6A66A51808}">
-  <dimension ref="A2:S45"/>
+  <dimension ref="A2:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="73" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="22" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" customWidth="1"/>
+    <col min="2" max="22" width="18.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
         <v>37</v>
       </c>
@@ -958,7 +968,7 @@
       <c r="F2" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="24" t="s">
         <v>45</v>
       </c>
       <c r="I2" s="31" t="s">
@@ -968,20 +978,20 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B3" s="37" t="s">
         <v>9</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F3" s="25">
         <v>4.96</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="25">
         <f>F3*5000*25</f>
         <v>620000</v>
       </c>
@@ -989,8 +999,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B4" s="37" t="s">
         <v>62</v>
       </c>
       <c r="C4">
@@ -999,13 +1009,12 @@
       <c r="D4">
         <v>40</v>
       </c>
-      <c r="F4" s="25"/>
       <c r="K4" s="29" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B5" s="37" t="s">
         <v>35</v>
       </c>
       <c r="C5">
@@ -1015,120 +1024,95 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E8" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B9" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C9" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D9" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E9" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F9" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="G9" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H9" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I9" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="J9" s="21" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C11" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="3">
-        <v>1</v>
-      </c>
-      <c r="E10" s="26">
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="26">
         <v>0</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="F11" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="27" t="s">
+      <c r="G11" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="27">
+      <c r="H11" s="27">
         <v>5000</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="28" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B12" s="28" t="s">
         <v>11</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="23" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E11" s="23">
-        <v>32</v>
-      </c>
-      <c r="F11" s="23">
-        <v>255</v>
-      </c>
-      <c r="G11" s="22">
-        <v>33</v>
-      </c>
-      <c r="H11" s="22">
-        <v>255</v>
-      </c>
-      <c r="I11" s="21">
-        <v>38</v>
-      </c>
-      <c r="J11" s="21">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="20" t="s">
-        <v>13</v>
       </c>
       <c r="C12" s="30" t="s">
         <v>10</v>
@@ -1138,13 +1122,13 @@
         <v>1</v>
       </c>
       <c r="E12" s="23">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F12" s="23">
         <v>255</v>
       </c>
       <c r="G12" s="22">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H12" s="22">
         <v>255</v>
@@ -1153,118 +1137,118 @@
         <v>38</v>
       </c>
       <c r="J12" s="21">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B13" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="23" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E13" s="23">
+        <v>34</v>
+      </c>
+      <c r="F13" s="23">
+        <v>255</v>
+      </c>
+      <c r="G13" s="22">
+        <v>35</v>
+      </c>
+      <c r="H13" s="22">
+        <v>255</v>
+      </c>
+      <c r="I13" s="21">
+        <v>38</v>
+      </c>
+      <c r="J13" s="21">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C15" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D15" s="3">
         <v>0</v>
       </c>
-      <c r="E14" s="26">
-        <v>1</v>
-      </c>
-      <c r="F14" s="27" t="s">
+      <c r="E15" s="26">
+        <v>1</v>
+      </c>
+      <c r="F15" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G14" s="27" t="s">
+      <c r="G15" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="H14" s="27">
+      <c r="H15" s="27">
         <v>5000</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="28" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B16" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C16" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="23" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E15" s="23">
+      <c r="D16" s="23" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E16" s="23">
         <v>36</v>
       </c>
-      <c r="F15" s="23">
-        <v>255</v>
-      </c>
-      <c r="G15" s="22">
+      <c r="F16" s="23">
+        <v>255</v>
+      </c>
+      <c r="G16" s="22">
         <v>37</v>
       </c>
-      <c r="H15" s="22">
-        <v>255</v>
-      </c>
-      <c r="I15" s="21">
+      <c r="H16" s="22">
+        <v>255</v>
+      </c>
+      <c r="I16" s="21">
         <v>39</v>
       </c>
-      <c r="J15" s="21">
+      <c r="J16" s="21">
         <v>240</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C18" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="3">
-        <v>1</v>
-      </c>
-      <c r="E17" s="26">
+      <c r="D18" s="3">
+        <v>1</v>
+      </c>
+      <c r="E18" s="26">
         <v>2</v>
       </c>
-      <c r="F17" s="27" t="s">
+      <c r="F18" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G17" s="27" t="s">
+      <c r="G18" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="H17" s="27">
+      <c r="H18" s="27">
         <v>5000</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="28" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B19" s="28" t="s">
         <v>11</v>
-      </c>
-      <c r="C18" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="23" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E18" s="23">
-        <v>52</v>
-      </c>
-      <c r="F18" s="23">
-        <v>255</v>
-      </c>
-      <c r="G18" s="22">
-        <v>53</v>
-      </c>
-      <c r="H18" s="22">
-        <v>255</v>
-      </c>
-      <c r="I18" s="21">
-        <v>58</v>
-      </c>
-      <c r="J18" s="21">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="20" t="s">
-        <v>13</v>
       </c>
       <c r="C19" s="30" t="s">
         <v>10</v>
@@ -1274,13 +1258,13 @@
         <v>1</v>
       </c>
       <c r="E19" s="23">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F19" s="23">
         <v>255</v>
       </c>
       <c r="G19" s="22">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H19" s="22">
         <v>255</v>
@@ -1289,12 +1273,12 @@
         <v>58</v>
       </c>
       <c r="J19" s="21">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="29" t="s">
-        <v>12</v>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B20" s="20" t="s">
+        <v>13</v>
       </c>
       <c r="C20" s="30" t="s">
         <v>10</v>
@@ -1304,13 +1288,13 @@
         <v>1</v>
       </c>
       <c r="E20" s="23">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F20" s="23">
         <v>255</v>
       </c>
       <c r="G20" s="22">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H20" s="22">
         <v>255</v>
@@ -1319,65 +1303,65 @@
         <v>58</v>
       </c>
       <c r="J20" s="21">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B21" s="29" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
+      <c r="C21" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="23" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E21" s="23">
+        <v>56</v>
+      </c>
+      <c r="F21" s="23">
+        <v>255</v>
+      </c>
+      <c r="G21" s="22">
+        <v>57</v>
+      </c>
+      <c r="H21" s="22">
+        <v>255</v>
+      </c>
+      <c r="I21" s="21">
+        <v>58</v>
+      </c>
+      <c r="J21" s="21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B23" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C23" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D23" s="3">
         <v>2</v>
       </c>
-      <c r="E22" s="26">
-        <v>1</v>
-      </c>
-      <c r="F22" s="27" t="s">
+      <c r="E23" s="26">
+        <v>1</v>
+      </c>
+      <c r="F23" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G22" s="27" t="s">
+      <c r="G23" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="H22" s="27">
+      <c r="H23" s="27">
         <v>2500</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="28" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B24" s="28" t="s">
         <v>11</v>
-      </c>
-      <c r="C23" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="23" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E23" s="23">
-        <v>59</v>
-      </c>
-      <c r="F23" s="23">
-        <v>255</v>
-      </c>
-      <c r="G23" s="22">
-        <v>60</v>
-      </c>
-      <c r="H23" s="22">
-        <v>255</v>
-      </c>
-      <c r="I23" s="21">
-        <v>63</v>
-      </c>
-      <c r="J23" s="21">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="20" t="s">
-        <v>13</v>
       </c>
       <c r="C24" s="30" t="s">
         <v>14</v>
@@ -1387,13 +1371,13 @@
         <v>1</v>
       </c>
       <c r="E24" s="23">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F24" s="23">
         <v>255</v>
       </c>
       <c r="G24" s="22">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H24" s="22">
         <v>255</v>
@@ -1402,99 +1386,99 @@
         <v>63</v>
       </c>
       <c r="J24" s="21">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B25" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="23" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E25" s="23">
+        <v>61</v>
+      </c>
+      <c r="F25" s="23">
+        <v>255</v>
+      </c>
+      <c r="G25" s="22">
+        <v>62</v>
+      </c>
+      <c r="H25" s="22">
+        <v>255</v>
+      </c>
+      <c r="I25" s="21">
+        <v>63</v>
+      </c>
+      <c r="J25" s="21">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="29" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" s="5"/>
+      <c r="B26" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="30" t="s">
+      <c r="C26" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="23" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E25" s="23">
+      <c r="D26" s="23" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E26" s="23">
         <v>59</v>
       </c>
-      <c r="F25" s="23">
-        <v>255</v>
-      </c>
-      <c r="G25" s="22">
+      <c r="F26" s="23">
+        <v>255</v>
+      </c>
+      <c r="G26" s="22">
         <v>60</v>
       </c>
-      <c r="H25" s="22">
-        <v>255</v>
-      </c>
-      <c r="I25" s="21">
+      <c r="H26" s="22">
+        <v>255</v>
+      </c>
+      <c r="I26" s="21">
         <v>61</v>
       </c>
-      <c r="J25" s="21">
+      <c r="J26" s="21">
         <v>240</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27" s="5"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B28" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" s="3">
+      <c r="C28" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="3">
         <v>0</v>
       </c>
-      <c r="E27" s="26">
+      <c r="E28" s="26">
         <v>2</v>
       </c>
-      <c r="F27" s="27" t="s">
+      <c r="F28" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="27" t="s">
+      <c r="G28" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="H27" s="27">
+      <c r="H28" s="27">
         <v>5000</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="28" t="s">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B29" s="28" t="s">
         <v>11</v>
-      </c>
-      <c r="C28" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="23" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E28" s="23">
-        <v>12</v>
-      </c>
-      <c r="F28" s="23">
-        <v>255</v>
-      </c>
-      <c r="G28" s="22">
-        <v>13</v>
-      </c>
-      <c r="H28" s="22">
-        <v>255</v>
-      </c>
-      <c r="I28" s="21">
-        <v>14</v>
-      </c>
-      <c r="J28" s="21">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="20" t="s">
-        <v>13</v>
       </c>
       <c r="C29" s="30" t="s">
         <v>10</v>
@@ -1504,27 +1488,27 @@
         <v>1</v>
       </c>
       <c r="E29" s="23">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F29" s="23">
         <v>255</v>
       </c>
       <c r="G29" s="22">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H29" s="22">
         <v>255</v>
       </c>
       <c r="I29" s="21">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J29" s="21">
         <v>255</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="29" t="s">
-        <v>12</v>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B30" s="20" t="s">
+        <v>13</v>
       </c>
       <c r="C30" s="30" t="s">
         <v>10</v>
@@ -1534,77 +1518,83 @@
         <v>1</v>
       </c>
       <c r="E30" s="23">
+        <v>15</v>
+      </c>
+      <c r="F30" s="23">
+        <v>255</v>
+      </c>
+      <c r="G30" s="22">
+        <v>16</v>
+      </c>
+      <c r="H30" s="22">
+        <v>255</v>
+      </c>
+      <c r="I30" s="21">
+        <v>17</v>
+      </c>
+      <c r="J30" s="21">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B31" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="23" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E31" s="23">
         <v>18</v>
       </c>
-      <c r="F30" s="23">
-        <v>255</v>
-      </c>
-      <c r="G30" s="22">
+      <c r="F31" s="23">
+        <v>255</v>
+      </c>
+      <c r="G31" s="22">
         <v>19</v>
       </c>
-      <c r="H30" s="22">
-        <v>255</v>
-      </c>
-      <c r="I30" s="21">
+      <c r="H31" s="22">
+        <v>255</v>
+      </c>
+      <c r="I31" s="21">
         <v>20</v>
       </c>
-      <c r="J30" s="21">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="3" t="s">
+      <c r="J31" s="21">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B33" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C32" s="26" t="s">
+      <c r="C33" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="3">
-        <v>1</v>
-      </c>
-      <c r="E32" s="26">
+      <c r="D33" s="3">
+        <v>1</v>
+      </c>
+      <c r="E33" s="26">
         <v>2</v>
       </c>
-      <c r="F32" s="27" t="s">
+      <c r="F33" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G32" s="27" t="s">
+      <c r="G33" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="H32" s="27">
+      <c r="H33" s="27">
         <v>2500</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B33" s="28" t="s">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B34" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="30" t="s">
+      <c r="C34" s="30" t="s">
         <v>16</v>
-      </c>
-      <c r="D33" s="23" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E33" s="23">
-        <v>78</v>
-      </c>
-      <c r="F33" s="23">
-        <v>255</v>
-      </c>
-      <c r="G33" s="21">
-        <v>79</v>
-      </c>
-      <c r="H33" s="21">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B34" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" s="30" t="s">
-        <v>17</v>
       </c>
       <c r="D34" s="23" t="b">
         <f>FALSE()</f>
@@ -1623,281 +1613,176 @@
         <v>240</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B36" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D36" s="3">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B35" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="23" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E36" s="3">
-        <v>0</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E35" s="23">
+        <v>78</v>
+      </c>
+      <c r="F35" s="23">
+        <v>255</v>
+      </c>
+      <c r="G35" s="21">
+        <v>79</v>
+      </c>
+      <c r="H35" s="21">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B38" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D38" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38" s="3">
         <v>0</v>
       </c>
       <c r="F38" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B40" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B40" s="3" t="s">
+      <c r="D40" s="3">
+        <v>1</v>
+      </c>
+      <c r="E40" s="3">
+        <v>0</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B42" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D40" s="3">
-        <v>1</v>
-      </c>
-      <c r="E40" s="3">
-        <v>1</v>
-      </c>
-      <c r="F40" s="3" t="s">
+      <c r="D42" s="3">
+        <v>1</v>
+      </c>
+      <c r="E42" s="3">
+        <v>1</v>
+      </c>
+      <c r="F42" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>22</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B44" t="s">
         <v>38</v>
       </c>
-      <c r="C42" s="32" t="s">
+      <c r="C44" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D42" s="33" t="s">
+      <c r="D44" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="E42" s="33" t="s">
+      <c r="E44" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="F42" s="33" t="s">
+      <c r="F44" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="G42" s="34" t="s">
+      <c r="G44" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="H42" s="34" t="s">
+      <c r="H44" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="I42" s="35" t="s">
+      <c r="I44" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="J42" s="35" t="s">
+      <c r="J44" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="K42" s="35" t="s">
+      <c r="K44" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="L42" s="35" t="s">
+      <c r="L44" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="M42" s="35" t="s">
+      <c r="M44" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="N42" s="36" t="s">
+      <c r="N44" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="O42" s="36" t="s">
+      <c r="O44" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="P42" s="36" t="s">
+      <c r="P44" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="Q42" s="36" t="s">
+      <c r="Q44" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="R42" s="35" t="s">
+      <c r="R44" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="S42" s="35" t="s">
+      <c r="S44" s="35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
         <v>2</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C45" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D43" s="12">
+      <c r="D45" s="12">
         <v>129</v>
       </c>
-      <c r="E43" s="12">
+      <c r="E45" s="12">
         <v>11</v>
       </c>
-      <c r="F43" s="1">
+      <c r="F45" s="1">
         <v>12500</v>
       </c>
-      <c r="G43" s="6">
+      <c r="G45" s="6">
         <v>39</v>
       </c>
-      <c r="H43" s="6">
+      <c r="H45" s="6">
         <v>15</v>
       </c>
-      <c r="I43" s="9" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="J43" s="8" t="b">
+      <c r="I45" s="9" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J45" s="8" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="K43" s="8" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L43" s="8" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M43" s="8" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="N43" s="8" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="O43" s="8" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="P43" s="8" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="Q43" s="8" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="R43" s="16" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="S43" s="18" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>1</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D44" s="1">
-        <v>18</v>
-      </c>
-      <c r="E44" s="12">
-        <v>11</v>
-      </c>
-      <c r="F44" s="1">
-        <v>25000</v>
-      </c>
-      <c r="G44" s="6">
-        <v>21</v>
-      </c>
-      <c r="H44" s="6">
-        <v>255</v>
-      </c>
-      <c r="I44" s="9" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="J44" s="8" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K44" s="8" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L44" s="8" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M44" s="8" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="N44" s="8" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="O44" s="8" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="P44" s="8" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="Q44" s="8" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="R44" s="16" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="S44" s="18" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D45" s="15">
-        <v>51</v>
-      </c>
-      <c r="E45" s="15">
-        <v>11</v>
-      </c>
-      <c r="F45" s="2">
-        <v>25000</v>
-      </c>
-      <c r="G45" s="7">
-        <v>63</v>
-      </c>
-      <c r="H45" s="7">
-        <v>255</v>
-      </c>
-      <c r="I45" s="10" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="J45" s="11" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K45" s="11" t="b">
+      <c r="K45" s="8" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
@@ -1905,31 +1790,165 @@
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="M45" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="N45" s="11" t="b">
+      <c r="M45" s="8" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N45" s="8" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="O45" s="8" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="P45" s="8" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="Q45" s="8" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="R45" s="16" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="S45" s="18" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="O45" s="11" t="b">
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="1">
+        <v>18</v>
+      </c>
+      <c r="E46" s="12">
+        <v>11</v>
+      </c>
+      <c r="F46" s="1">
+        <v>25000</v>
+      </c>
+      <c r="G46" s="6">
+        <v>21</v>
+      </c>
+      <c r="H46" s="6">
+        <v>255</v>
+      </c>
+      <c r="I46" s="9" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J46" s="8" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K46" s="8" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="P45" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="Q45" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="R45" s="17" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="S45" s="19" t="b">
+      <c r="L46" s="8" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M46" s="8" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N46" s="8" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="O46" s="8" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="P46" s="8" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="Q46" s="8" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="R46" s="16" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="S46" s="18" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" s="15">
+        <v>51</v>
+      </c>
+      <c r="E47" s="15">
+        <v>11</v>
+      </c>
+      <c r="F47" s="2">
+        <v>25000</v>
+      </c>
+      <c r="G47" s="7">
+        <v>63</v>
+      </c>
+      <c r="H47" s="7">
+        <v>255</v>
+      </c>
+      <c r="I47" s="10" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J47" s="11" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K47" s="11" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L47" s="8" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M47" s="11" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N47" s="11" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O47" s="11" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="P47" s="11" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="Q47" s="11" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="R47" s="17" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="S47" s="19" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
@@ -1939,29 +1958,12 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="J44 M45" formula="1"/>
+    <ignoredError sqref="J46 M47" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3be8e3c0-2842-4b5c-b060-a331e5ce9465" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010085EDC4FCBFEAC44C90B472F1F1C900EA" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e45273375250329c822a0a405177b348">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3be8e3c0-2842-4b5c-b060-a331e5ce9465" xmlns:ns4="6b4e13fc-0909-4af8-88c8-1f82cb55b253" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a0e1ca657407e685f067414fb59c7721" ns3:_="" ns4:_="">
     <xsd:import namespace="3be8e3c0-2842-4b5c-b060-a331e5ce9465"/>
@@ -2190,10 +2192,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3be8e3c0-2842-4b5c-b060-a331e5ce9465" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B746C5C-9FCE-47B1-9B21-C70DB5E5E0E1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{917E079B-BC71-4494-9E92-79C803C2F6BC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3be8e3c0-2842-4b5c-b060-a331e5ce9465"/>
+    <ds:schemaRef ds:uri="6b4e13fc-0909-4af8-88c8-1f82cb55b253"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2216,20 +2246,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{917E079B-BC71-4494-9E92-79C803C2F6BC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B746C5C-9FCE-47B1-9B21-C70DB5E5E0E1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3be8e3c0-2842-4b5c-b060-a331e5ce9465"/>
-    <ds:schemaRef ds:uri="6b4e13fc-0909-4af8-88c8-1f82cb55b253"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Moved scrolling plot widget to plotting.py
</commit_message>
<xml_diff>
--- a/lib/VortexTest.xlsx
+++ b/lib/VortexTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayash\Programming\vortex_parser\lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49A99E6-4363-49D0-8CFF-B84F3ECC7048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E47A96-166E-435E-A9E9-9E0055CD173B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="522" xr2:uid="{93DD1A3E-79F5-40A0-9DE4-B4C0229D9C52}"/>
   </bookViews>
@@ -967,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7758D255-7225-412E-BCCB-5D6A66A51808}">
-  <dimension ref="A2:S48"/>
+  <dimension ref="A2:S47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1731,94 +1731,161 @@
         <v>63</v>
       </c>
     </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="E44" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="F44" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="G44" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="H44" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="I44" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="J44" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="K44" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="L44" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="M44" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="N44" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="O44" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="P44" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q44" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="R44" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="S44" s="35" t="s">
+        <v>34</v>
+      </c>
+    </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>22</v>
-      </c>
       <c r="B45" t="s">
-        <v>38</v>
-      </c>
-      <c r="C45" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="D45" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="E45" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="F45" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="G45" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="H45" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" s="12">
+        <v>131</v>
+      </c>
+      <c r="E45" s="12">
+        <v>11</v>
+      </c>
+      <c r="F45" s="1">
+        <v>12500</v>
+      </c>
+      <c r="G45" s="6">
+        <v>39</v>
+      </c>
+      <c r="H45" s="6">
+        <v>15</v>
+      </c>
+      <c r="I45" s="9" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J45" s="8" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I45" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="J45" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="K45" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="L45" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="M45" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="N45" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="O45" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="P45" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q45" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="R45" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="S45" s="35" t="s">
-        <v>34</v>
+      <c r="K45" s="8" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L45" s="8" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M45" s="8" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N45" s="8" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="O45" s="8" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="P45" s="8" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="Q45" s="8" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="R45" s="16" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="S45" s="18" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C46" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D46" s="12">
-        <v>131</v>
+      <c r="D46" s="38">
+        <v>18</v>
       </c>
       <c r="E46" s="12">
         <v>11</v>
       </c>
       <c r="F46" s="1">
-        <v>12500</v>
+        <v>25000</v>
       </c>
       <c r="G46" s="6">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="H46" s="6">
-        <v>15</v>
+        <v>255</v>
       </c>
       <c r="I46" s="9" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="J46" s="8" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="K46" s="8" t="b">
         <f>FALSE()</f>
@@ -1857,136 +1924,69 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>1</v>
-      </c>
-      <c r="C47" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D47" s="38">
-        <v>18</v>
-      </c>
-      <c r="E47" s="12">
+        <v>3</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" s="15">
+        <v>51</v>
+      </c>
+      <c r="E47" s="15">
         <v>11</v>
       </c>
-      <c r="F47" s="1">
+      <c r="F47" s="2">
         <v>25000</v>
       </c>
-      <c r="G47" s="6">
-        <v>21</v>
-      </c>
-      <c r="H47" s="6">
-        <v>255</v>
-      </c>
-      <c r="I47" s="9" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="J47" s="8" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K47" s="8" t="b">
+      <c r="G47" s="7">
+        <v>63</v>
+      </c>
+      <c r="H47" s="7">
+        <v>255</v>
+      </c>
+      <c r="I47" s="10" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J47" s="11" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="L47" s="8" t="b">
+      <c r="K47" s="11" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="M47" s="8" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="N47" s="8" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="O47" s="8" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="P47" s="8" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="Q47" s="8" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="R47" s="16" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="S47" s="18" t="b">
+      <c r="L47" s="11" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
-        <v>3</v>
-      </c>
-      <c r="C48" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D48" s="15">
-        <v>51</v>
-      </c>
-      <c r="E48" s="15">
-        <v>11</v>
-      </c>
-      <c r="F48" s="2">
-        <v>25000</v>
-      </c>
-      <c r="G48" s="7">
-        <v>63</v>
-      </c>
-      <c r="H48" s="7">
-        <v>255</v>
-      </c>
-      <c r="I48" s="10" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="J48" s="11" t="b">
+      <c r="M47" s="11" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N47" s="11" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="K48" s="11" t="b">
+      <c r="O47" s="11" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="L48" s="11" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M48" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="N48" s="11" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O48" s="11" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P48" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="Q48" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="R48" s="17" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="S48" s="19" t="b">
+      <c r="P47" s="11" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="Q47" s="11" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="R47" s="17" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="S47" s="19" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
@@ -1996,29 +1996,12 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="J47 M48" formula="1"/>
+    <ignoredError sqref="J46 M47" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3be8e3c0-2842-4b5c-b060-a331e5ce9465" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010085EDC4FCBFEAC44C90B472F1F1C900EA" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e45273375250329c822a0a405177b348">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3be8e3c0-2842-4b5c-b060-a331e5ce9465" xmlns:ns4="6b4e13fc-0909-4af8-88c8-1f82cb55b253" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a0e1ca657407e685f067414fb59c7721" ns3:_="" ns4:_="">
     <xsd:import namespace="3be8e3c0-2842-4b5c-b060-a331e5ce9465"/>
@@ -2247,10 +2230,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3be8e3c0-2842-4b5c-b060-a331e5ce9465" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B746C5C-9FCE-47B1-9B21-C70DB5E5E0E1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{917E079B-BC71-4494-9E92-79C803C2F6BC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3be8e3c0-2842-4b5c-b060-a331e5ce9465"/>
+    <ds:schemaRef ds:uri="6b4e13fc-0909-4af8-88c8-1f82cb55b253"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2273,20 +2284,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{917E079B-BC71-4494-9E92-79C803C2F6BC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B746C5C-9FCE-47B1-9B21-C70DB5E5E0E1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3be8e3c0-2842-4b5c-b060-a331e5ce9465"/>
-    <ds:schemaRef ds:uri="6b4e13fc-0909-4af8-88c8-1f82cb55b253"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>